<commit_message>
bugfixes and serbian additions
</commit_message>
<xml_diff>
--- a/Plans/Serbian Extra Focuses.xlsx
+++ b/Plans/Serbian Extra Focuses.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
@@ -18,10 +18,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Forfatter</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="O2" authorId="0" shapeId="0">
+    <comment ref="O2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -31,7 +31,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Forfatter:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -45,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="0" shapeId="0">
+    <comment ref="O3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +55,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Forfatter:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -69,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O4" authorId="0" shapeId="0">
+    <comment ref="O4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +79,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Forfatter:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -93,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -103,7 +103,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Forfatter:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -117,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O5" authorId="0" shapeId="0">
+    <comment ref="O5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +127,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Forfatter:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Nedic's Army Reform</t>
   </si>
@@ -175,9 +175,6 @@
     <t>Invest in Railroads</t>
   </si>
   <si>
-    <t>Kosovo Chromium</t>
-  </si>
-  <si>
     <t>Control Over Villages</t>
   </si>
   <si>
@@ -201,11 +198,17 @@
   <si>
     <t>Markov Plan - Cheaper Rifles and Motorized Equipment</t>
   </si>
+  <si>
+    <t>Russian Refugees</t>
+  </si>
+  <si>
+    <t>Kovovo Chromium</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -358,7 +361,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperkobling" xfId="2" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -376,7 +379,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -418,7 +421,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -451,26 +454,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -503,23 +489,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -699,10 +668,10 @@
   <dimension ref="B1:X6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:R2"/>
+      <selection activeCell="F5" sqref="F5:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.140625" defaultRowHeight="75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="7.140625" style="19"/>
   </cols>
@@ -721,7 +690,7 @@
       </c>
       <c r="R1" s="21"/>
       <c r="T1" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U1" s="20"/>
       <c r="V1" s="20"/>
@@ -746,7 +715,7 @@
       <c r="Q2" s="21"/>
       <c r="R2" s="21"/>
       <c r="T2" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U2" s="20"/>
       <c r="V2" s="20"/>
@@ -765,13 +734,13 @@
       <c r="M3" s="21"/>
       <c r="N3" s="21"/>
       <c r="O3" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P3" s="20"/>
       <c r="Q3" s="21"/>
       <c r="R3" s="21"/>
       <c r="T3" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U3" s="20"/>
       <c r="V3" s="20"/>
@@ -782,10 +751,12 @@
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
       <c r="D4" s="20" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E4" s="20"/>
-      <c r="F4" s="21"/>
+      <c r="F4" s="21" t="s">
+        <v>18</v>
+      </c>
       <c r="G4" s="21"/>
       <c r="M4" s="21"/>
       <c r="N4" s="21"/>
@@ -796,7 +767,7 @@
       <c r="Q4" s="21"/>
       <c r="R4" s="21"/>
       <c r="T4" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U4" s="20"/>
       <c r="V4" s="20"/>
@@ -807,7 +778,7 @@
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
       <c r="D5" s="20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="20"/>
       <c r="F5" s="21"/>
@@ -823,13 +794,13 @@
     </row>
     <row r="6" spans="2:24" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D6" s="21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="21"/>
       <c r="M6" s="21"/>
       <c r="N6" s="21"/>
       <c r="O6" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P6" s="20"/>
       <c r="Q6" s="21"/>
@@ -837,11 +808,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="T1:X1"/>
-    <mergeCell ref="T2:X2"/>
-    <mergeCell ref="T3:X3"/>
-    <mergeCell ref="T4:X4"/>
-    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q6:R6"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
@@ -852,25 +836,12 @@
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F5:G5"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q6:R6"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="T1:X1"/>
+    <mergeCell ref="T2:X2"/>
+    <mergeCell ref="T3:X3"/>
+    <mergeCell ref="T4:X4"/>
+    <mergeCell ref="Q5:R5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -886,7 +857,7 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.140625" customWidth="1"/>
     <col min="2" max="2" width="38.140625" customWidth="1"/>
@@ -13820,7 +13791,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>